<commit_message>
Added basic Board UI
1) Added basic Board UI

2) Updated Sprint 3 backlog
</commit_message>
<xml_diff>
--- a/sprints/sprint3/Sprint 3 Backlog Burndown.xlsx
+++ b/sprints/sprint3/Sprint 3 Backlog Burndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swamp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swamp\Desktop\CapstoneGroup3\sprints\sprint3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73ED0533-D5FD-4C36-8AB1-76D0A4B88A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4646DB-8B5D-4EB7-9FE1-D08E6EB92ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3585" yWindow="2850" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Related User Story</t>
   </si>
@@ -105,6 +105,21 @@
   </si>
   <si>
     <t>Assign task to a user in a group</t>
+  </si>
+  <si>
+    <t>Eman</t>
+  </si>
+  <si>
+    <t>Jacob</t>
+  </si>
+  <si>
+    <t>Create Edit Board UI</t>
+  </si>
+  <si>
+    <t>Fix approval rejection process</t>
+  </si>
+  <si>
+    <t>Jabesi</t>
   </si>
 </sst>
 </file>
@@ -402,7 +417,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$38:$H$38</c:f>
+              <c:f>Sheet1!$D$40:$H$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1169,7 +1184,7 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>171451</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1461,10 +1476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1521,7 +1536,9 @@
       <c r="B3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="D3" s="7"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -1535,7 +1552,9 @@
       <c r="B4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="8"/>
+      <c r="C4" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="D4" s="7"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -1544,8 +1563,12 @@
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+      <c r="B5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="D5" s="7"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -1553,25 +1576,25 @@
       <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
+      <c r="A7" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="B7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="10"/>
+        <v>16</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>24</v>
+      </c>
       <c r="D7" s="10"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -1581,9 +1604,11 @@
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="10"/>
+        <v>25</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>24</v>
+      </c>
       <c r="D8" s="10"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -1593,7 +1618,7 @@
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -1604,7 +1629,9 @@
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
+      <c r="B10" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="9"/>
@@ -1613,34 +1640,34 @@
       <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
+      <c r="A13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="9"/>
@@ -1649,20 +1676,22 @@
       <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
@@ -1699,20 +1728,20 @@
       <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -1720,7 +1749,7 @@
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="9"/>
@@ -1728,29 +1757,29 @@
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
     </row>
-    <row r="22" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-    </row>
-    <row r="23" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
+    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+    </row>
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
-      <c r="B24" s="16"/>
+      <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
       <c r="E24" s="14"/>
@@ -1768,30 +1797,30 @@
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
+    <row r="26" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+    </row>
+    <row r="27" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="15"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
       <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
+      <c r="C28" s="18"/>
       <c r="D28" s="17"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
@@ -1801,7 +1830,7 @@
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="17"/>
       <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
+      <c r="C29" s="18"/>
       <c r="D29" s="17"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
@@ -1809,20 +1838,20 @@
       <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
@@ -1869,50 +1898,70 @@
       <c r="H35" s="9"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
+      <c r="A36" s="20"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
+      <c r="A37" s="20"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="2" t="s">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1">
-        <f>SUM(D3:D37)</f>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1">
+        <f>SUM(D3:D39)</f>
         <v>0</v>
       </c>
-      <c r="E38" s="1">
-        <f t="shared" ref="E38:H38" si="0">SUM(E3:E37)</f>
+      <c r="E40" s="1">
+        <f t="shared" ref="E40:H40" si="0">SUM(E3:E39)</f>
         <v>0</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F40" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G38" s="1">
+      <c r="G40" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H38" s="1">
+      <c r="H40" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1932,12 +1981,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B208BF211488B4F880DF934C5C83A74" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0ea6ebcb2e074b139db49da06cf4ed1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bb8530a4-d58a-4eb7-b41a-d2b9ee1ee59d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71b55cd54d0ee2f4121790f6a497c1d7" ns2:_="">
     <xsd:import namespace="bb8530a4-d58a-4eb7-b41a-d2b9ee1ee59d"/>
@@ -2081,6 +2124,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2091,15 +2140,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D5C3914-7DAF-4B4D-BA97-A88E18DCB9DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2117,6 +2157,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50A4F540-0AB9-43E5-9CA4-0E2ADF00CD9E}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Added Board UI Changes
1) Added Board page link and UI changes
</commit_message>
<xml_diff>
--- a/sprints/sprint3/Sprint 3 Backlog Burndown.xlsx
+++ b/sprints/sprint3/Sprint 3 Backlog Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swamp\Desktop\CapstoneGroup3\sprints\sprint3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4646DB-8B5D-4EB7-9FE1-D08E6EB92ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9988F51-24DE-4535-A295-6C5672116066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3585" yWindow="2850" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Related User Story</t>
   </si>
@@ -1479,7 +1479,7 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1632,7 +1632,9 @@
       <c r="B10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="10"/>
+      <c r="C10" s="10" t="s">
+        <v>24</v>
+      </c>
       <c r="D10" s="10"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -1981,6 +1983,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B208BF211488B4F880DF934C5C83A74" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0ea6ebcb2e074b139db49da06cf4ed1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bb8530a4-d58a-4eb7-b41a-d2b9ee1ee59d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71b55cd54d0ee2f4121790f6a497c1d7" ns2:_="">
     <xsd:import namespace="bb8530a4-d58a-4eb7-b41a-d2b9ee1ee59d"/>
@@ -2124,12 +2132,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2140,6 +2142,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D5C3914-7DAF-4B4D-BA97-A88E18DCB9DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2157,15 +2168,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50A4F540-0AB9-43E5-9CA4-0E2ADF00CD9E}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Updated Sprint Backlog for Sprint 3
1) Updated sb for sprint 3 with results
</commit_message>
<xml_diff>
--- a/sprints/sprint3/Sprint 3 Backlog Burndown.xlsx
+++ b/sprints/sprint3/Sprint 3 Backlog Burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swamp\Desktop\CapstoneGroup3\sprints\sprint3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9988F51-24DE-4535-A295-6C5672116066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2357987E-03CB-4255-A529-7740221D6046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3585" yWindow="2850" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>Related User Story</t>
   </si>
@@ -89,37 +89,43 @@
     <t>Create Board UI</t>
   </si>
   <si>
-    <t>Create Board Task UI</t>
-  </si>
-  <si>
-    <t>Edit Board functionality (adding/renaming columns)</t>
-  </si>
-  <si>
-    <t>Adding/Editing Task to Board functionality</t>
-  </si>
-  <si>
     <t>Assignments</t>
   </si>
   <si>
     <t>Assign stage of board to a group</t>
   </si>
   <si>
-    <t>Assign task to a user in a group</t>
-  </si>
-  <si>
     <t>Eman</t>
   </si>
   <si>
     <t>Jacob</t>
   </si>
   <si>
-    <t>Create Edit Board UI</t>
-  </si>
-  <si>
     <t>Fix approval rejection process</t>
   </si>
   <si>
     <t>Jabesi</t>
+  </si>
+  <si>
+    <t>Permissions</t>
+  </si>
+  <si>
+    <t>Add column</t>
+  </si>
+  <si>
+    <t>Delete Column</t>
+  </si>
+  <si>
+    <t>Rename Column</t>
+  </si>
+  <si>
+    <t>Create Edit Board UI (CRUD)</t>
+  </si>
+  <si>
+    <t>Implement board permissions</t>
+  </si>
+  <si>
+    <t>Reorder Column</t>
   </si>
 </sst>
 </file>
@@ -422,10 +428,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>20.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1479,19 +1485,19 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" customWidth="1"/>
-    <col min="2" max="2" width="122" customWidth="1"/>
+    <col min="1" max="1" width="34.453125" customWidth="1"/>
+    <col min="2" max="2" width="54.81640625" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="7.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -1511,7 +1517,7 @@
       <c r="G1" s="21"/>
       <c r="H1" s="21"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -1529,23 +1535,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>24</v>
-      </c>
+      <c r="C3" s="8"/>
       <c r="D3" s="7"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -1553,7 +1557,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="9"/>
@@ -1561,13 +1565,13 @@
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
       <c r="B5" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="9"/>
@@ -1575,7 +1579,7 @@
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1585,7 +1589,7 @@
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>15</v>
       </c>
@@ -1593,103 +1597,153 @@
         <v>16</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
+        <v>20</v>
+      </c>
+      <c r="D7" s="10">
+        <v>4</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10"/>
       <c r="B8" s="10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+        <v>20</v>
+      </c>
+      <c r="D8" s="10">
+        <v>4</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0</v>
+      </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10"/>
       <c r="B9" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
+        <v>24</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="10">
+        <v>5</v>
+      </c>
+      <c r="E9" s="9">
+        <v>3</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0</v>
+      </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10"/>
       <c r="B10" s="10" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+        <v>20</v>
+      </c>
+      <c r="D10" s="10">
+        <v>3</v>
+      </c>
+      <c r="E10" s="9">
+        <v>3</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0</v>
+      </c>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10"/>
       <c r="B11" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
+        <v>26</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="10">
+        <v>3</v>
+      </c>
+      <c r="E11" s="9">
+        <v>3</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0</v>
+      </c>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
+      <c r="B12" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="10">
+        <v>5</v>
+      </c>
+      <c r="E12" s="9">
+        <v>5</v>
+      </c>
+      <c r="F12" s="9">
+        <v>0</v>
+      </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="B14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
+        <v>18</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="11">
+        <v>8</v>
+      </c>
+      <c r="E14" s="9">
+        <v>6</v>
+      </c>
+      <c r="F14" s="9">
+        <v>0</v>
+      </c>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -1699,17 +1753,29 @@
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="E16" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="F16" s="9">
+        <v>0</v>
+      </c>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
@@ -1719,7 +1785,7 @@
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
     </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -1729,7 +1795,7 @@
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
     </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -1739,7 +1805,7 @@
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
     </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
@@ -1749,7 +1815,7 @@
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
     </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
       <c r="B21" s="13"/>
       <c r="C21" s="5"/>
@@ -1759,7 +1825,7 @@
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
     </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="B22" s="13"/>
       <c r="C22" s="5"/>
@@ -1769,7 +1835,7 @@
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
     </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1779,7 +1845,7 @@
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
     </row>
-    <row r="24" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -1789,7 +1855,7 @@
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
     </row>
-    <row r="25" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="15"/>
       <c r="B25" s="16"/>
       <c r="C25" s="15"/>
@@ -1799,7 +1865,7 @@
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
     </row>
-    <row r="26" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="15"/>
       <c r="B26" s="16"/>
       <c r="C26" s="15"/>
@@ -1809,7 +1875,7 @@
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
     </row>
-    <row r="27" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="15"/>
       <c r="B27" s="16"/>
       <c r="C27" s="15"/>
@@ -1819,7 +1885,7 @@
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A28" s="17"/>
       <c r="B28" s="17"/>
       <c r="C28" s="18"/>
@@ -1829,7 +1895,7 @@
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="17"/>
       <c r="B29" s="17"/>
       <c r="C29" s="18"/>
@@ -1839,7 +1905,7 @@
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A30" s="17"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
@@ -1849,7 +1915,7 @@
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A31" s="17"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
@@ -1859,7 +1925,7 @@
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A32" s="20"/>
       <c r="B32" s="20"/>
       <c r="C32" s="20"/>
@@ -1869,7 +1935,7 @@
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A33" s="20"/>
       <c r="B33" s="20"/>
       <c r="C33" s="20"/>
@@ -1879,7 +1945,7 @@
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A34" s="20"/>
       <c r="B34" s="20"/>
       <c r="C34" s="20"/>
@@ -1889,7 +1955,7 @@
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A35" s="20"/>
       <c r="B35" s="20"/>
       <c r="C35" s="20"/>
@@ -1899,7 +1965,7 @@
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
@@ -1909,7 +1975,7 @@
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
       <c r="C37" s="20"/>
@@ -1919,7 +1985,7 @@
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -1929,7 +1995,7 @@
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A39" s="6"/>
       <c r="B39" s="19" t="s">
         <v>9</v>
@@ -1941,7 +2007,7 @@
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
       <c r="B40" s="2" t="s">
         <v>10</v>
@@ -1949,11 +2015,11 @@
       <c r="C40" s="1"/>
       <c r="D40" s="1">
         <f>SUM(D3:D39)</f>
-        <v>0</v>
+        <v>32.5</v>
       </c>
       <c r="E40" s="1">
         <f t="shared" ref="E40:H40" si="0">SUM(E3:E39)</f>
-        <v>0</v>
+        <v>20.5</v>
       </c>
       <c r="F40" s="1">
         <f t="shared" si="0"/>
@@ -1983,12 +2049,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B208BF211488B4F880DF934C5C83A74" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0ea6ebcb2e074b139db49da06cf4ed1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bb8530a4-d58a-4eb7-b41a-d2b9ee1ee59d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71b55cd54d0ee2f4121790f6a497c1d7" ns2:_="">
     <xsd:import namespace="bb8530a4-d58a-4eb7-b41a-d2b9ee1ee59d"/>
@@ -2132,6 +2192,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2142,15 +2208,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D5C3914-7DAF-4B4D-BA97-A88E18DCB9DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2168,6 +2225,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50A4F540-0AB9-43E5-9CA4-0E2ADF00CD9E}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Updated the sprint doucmentation folder
1) Update the burndown with my worked hours
2) Uploaded the code coverage report
3) Added the wireframe used for the board
Re moved temp files
</commit_message>
<xml_diff>
--- a/sprints/sprint3/Sprint 3 Backlog Burndown.xlsx
+++ b/sprints/sprint3/Sprint 3 Backlog Burndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eo00037\source\repos\CapstoneGroup3\sprints\sprint3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ja00069\Downloads\CapstoneGroup3\sprints\sprint3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618A7EAF-61C3-41CA-BE81-D53659603B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08382362-D831-4EFA-847D-74DA33E7C212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="10368" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>Related User Story</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>Reorder Column</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t>Clean up project and documentation (doc strings)</t>
+  </si>
+  <si>
+    <t>Test missing branches on Project And user related classes</t>
   </si>
 </sst>
 </file>
@@ -428,10 +437,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>34.5</c:v>
+                  <c:v>49.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.5</c:v>
+                  <c:v>37.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1484,20 +1493,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" customWidth="1"/>
-    <col min="2" max="2" width="54.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="2" max="2" width="54.88671875" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="7.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -1517,7 +1526,7 @@
       <c r="G1" s="21"/>
       <c r="H1" s="21"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -1535,7 +1544,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>14</v>
       </c>
@@ -1549,7 +1558,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -1571,7 +1580,7 @@
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="7" t="s">
         <v>21</v>
@@ -1579,13 +1588,17 @@
       <c r="C5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="9"/>
+      <c r="D5" s="7">
+        <v>3</v>
+      </c>
+      <c r="E5" s="9">
+        <v>3</v>
+      </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1595,7 +1608,7 @@
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>15</v>
       </c>
@@ -1617,7 +1630,7 @@
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="10" t="s">
         <v>27</v>
@@ -1637,7 +1650,7 @@
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="10" t="s">
         <v>24</v>
@@ -1657,7 +1670,7 @@
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="10" t="s">
         <v>25</v>
@@ -1677,7 +1690,7 @@
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="10" t="s">
         <v>26</v>
@@ -1697,7 +1710,7 @@
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="10" t="s">
         <v>29</v>
@@ -1717,7 +1730,7 @@
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -1727,7 +1740,7 @@
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>17</v>
       </c>
@@ -1749,7 +1762,7 @@
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -1759,7 +1772,7 @@
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>23</v>
       </c>
@@ -1781,7 +1794,7 @@
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
@@ -1791,7 +1804,7 @@
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
     </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -1801,7 +1814,7 @@
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
     </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -1811,7 +1824,7 @@
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
     </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
@@ -1821,27 +1834,45 @@
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
     </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="9"/>
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="5">
+        <v>5</v>
+      </c>
+      <c r="E21" s="9">
+        <v>4</v>
+      </c>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
     </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="9"/>
+      <c r="B22" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="5">
+        <v>7</v>
+      </c>
+      <c r="E22" s="9">
+        <v>8</v>
+      </c>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
     </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1851,7 +1882,7 @@
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
     </row>
-    <row r="24" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -1861,7 +1892,7 @@
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
     </row>
-    <row r="25" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15"/>
       <c r="B25" s="16"/>
       <c r="C25" s="15"/>
@@ -1871,7 +1902,7 @@
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
     </row>
-    <row r="26" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15"/>
       <c r="B26" s="16"/>
       <c r="C26" s="15"/>
@@ -1881,7 +1912,7 @@
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
     </row>
-    <row r="27" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15"/>
       <c r="B27" s="16"/>
       <c r="C27" s="15"/>
@@ -1891,7 +1922,7 @@
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="17"/>
       <c r="B28" s="17"/>
       <c r="C28" s="18"/>
@@ -1901,7 +1932,7 @@
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" s="17"/>
       <c r="B29" s="17"/>
       <c r="C29" s="18"/>
@@ -1911,7 +1942,7 @@
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30" s="17"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
@@ -1921,7 +1952,7 @@
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" s="17"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
@@ -1931,7 +1962,7 @@
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" s="20"/>
       <c r="B32" s="20"/>
       <c r="C32" s="20"/>
@@ -1941,7 +1972,7 @@
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="20"/>
       <c r="B33" s="20"/>
       <c r="C33" s="20"/>
@@ -1951,7 +1982,7 @@
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A34" s="20"/>
       <c r="B34" s="20"/>
       <c r="C34" s="20"/>
@@ -1961,7 +1992,7 @@
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" s="20"/>
       <c r="B35" s="20"/>
       <c r="C35" s="20"/>
@@ -1971,7 +2002,7 @@
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
@@ -1981,7 +2012,7 @@
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
       <c r="C37" s="20"/>
@@ -1991,7 +2022,7 @@
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -2001,7 +2032,7 @@
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
       <c r="B39" s="19" t="s">
         <v>9</v>
@@ -2013,7 +2044,7 @@
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="2" t="s">
         <v>10</v>
@@ -2021,11 +2052,11 @@
       <c r="C40" s="1"/>
       <c r="D40" s="1">
         <f>SUM(D3:D39)</f>
-        <v>34.5</v>
+        <v>49.5</v>
       </c>
       <c r="E40" s="1">
         <f t="shared" ref="E40:H40" si="0">SUM(E3:E39)</f>
-        <v>22.5</v>
+        <v>37.5</v>
       </c>
       <c r="F40" s="1">
         <f t="shared" si="0"/>
@@ -2055,12 +2086,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B208BF211488B4F880DF934C5C83A74" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0ea6ebcb2e074b139db49da06cf4ed1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bb8530a4-d58a-4eb7-b41a-d2b9ee1ee59d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71b55cd54d0ee2f4121790f6a497c1d7" ns2:_="">
     <xsd:import namespace="bb8530a4-d58a-4eb7-b41a-d2b9ee1ee59d"/>
@@ -2204,6 +2229,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2214,15 +2245,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D5C3914-7DAF-4B4D-BA97-A88E18DCB9DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2240,6 +2262,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50A4F540-0AB9-43E5-9CA4-0E2ADF00CD9E}">
   <ds:schemaRefs>

</xml_diff>